<commit_message>
SCRPITs - DDL - DML - DQL
</commit_message>
<xml_diff>
--- a/Banco de Dados/Modelagem/GUFI-FÍSICO.xlsx
+++ b/Banco de Dados/Modelagem/GUFI-FÍSICO.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20377"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{3C35A107-2246-4AF4-9D34-33C021D901F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2C9F2C2-C8AF-47C2-ACE6-4387CCBD4B2B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E94712F-0F51-4F89-BFC9-2FE3FA142A83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -616,27 +616,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="51.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -647,7 +647,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -676,7 +676,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -705,7 +705,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -734,7 +734,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D5" s="2">
         <v>3</v>
       </c>
@@ -757,12 +757,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
@@ -779,7 +779,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>1</v>
       </c>
@@ -814,7 +814,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F11" s="1">
         <v>1</v>
       </c>
@@ -837,7 +837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E12" s="10"/>
       <c r="F12" s="2">
         <v>2</v>
@@ -861,10 +861,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>32</v>
       </c>
@@ -872,7 +872,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>33</v>
       </c>
@@ -892,7 +892,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -912,7 +912,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>2</v>
       </c>
@@ -932,7 +932,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F20" s="2">
         <v>3</v>
       </c>

</xml_diff>